<commit_message>
Substituição imagens e corrigindo mensagem de erro.
</commit_message>
<xml_diff>
--- a/erp-v2/assets/PLANILHA TESTE CONTRATO.xlsx
+++ b/erp-v2/assets/PLANILHA TESTE CONTRATO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hawly\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA479EE4-0B08-4BE4-8B4D-99928F49B0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642C2E97-849E-42AA-9E71-16D3B703881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
@@ -476,7 +476,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -487,14 +487,6 @@
       <c r="E3">
         <v>61.32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>